<commit_message>
Novos campos na planilha e nas funções python.
</commit_message>
<xml_diff>
--- a/monitorias.xlsx
+++ b/monitorias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,27 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>chamado</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>duracao</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>nome_cliente</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>categoria</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>nota</t>
         </is>
       </c>
     </row>
@@ -479,17 +489,19 @@
       <c r="C2" t="n">
         <v>321</v>
       </c>
-      <c r="D2" t="n">
-        <v>321</v>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>321</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>321</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Consulta</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -502,24 +514,62 @@
           <t>0123-03-12</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>123</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>123</v>
+      </c>
+      <c r="F3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Consulta</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1111-11-11</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Hardware</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adição do campo projeto.
</commit_message>
<xml_diff>
--- a/monitorias.xlsx
+++ b/monitorias.xlsx
@@ -1,37 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\monitorias\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9658E3C-1AF0-4D27-9A6E-D4DDEFC9555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>nome_analista</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>id_atendimento</t>
+  </si>
+  <si>
+    <t>chamado</t>
+  </si>
+  <si>
+    <t>duracao</t>
+  </si>
+  <si>
+    <t>nome_cliente</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>nota</t>
+  </si>
+  <si>
+    <t>projeto</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +90,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,157 +417,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>nome_analista</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>data</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>id_atendimento</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>chamado</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>duracao</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>nome_cliente</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>categoria</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>nota</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Guilherme</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1111-01-01</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>321</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>321</v>
-      </c>
-      <c r="F2" t="n">
-        <v>321</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Consulta</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0123-03-12</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>123</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>123</v>
-      </c>
-      <c r="F3" t="n">
-        <v>123</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Consulta</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Teste</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1111-11-11</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1111</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Hardware</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correção da tabela de monitorias
</commit_message>
<xml_diff>
--- a/monitorias.xlsx
+++ b/monitorias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\monitorias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3D9FA3-5325-4B85-A8C7-2A6B99248F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C673E67E-2B4C-4542-9C06-3FF2D0AADB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,26 +20,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>projeto</t>
+  </si>
   <si>
     <t>nome_analista</t>
   </si>
   <si>
-    <t>projeto</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>id_atendimento</t>
   </si>
   <si>
+    <t>duracao</t>
+  </si>
+  <si>
     <t>chamado</t>
   </si>
   <si>
-    <t>duracao</t>
-  </si>
-  <si>
     <t>nome_cliente</t>
   </si>
   <si>
@@ -49,7 +49,28 @@
     <t>nota</t>
   </si>
   <si>
-    <t>observação</t>
+    <t>2024-04-23</t>
+  </si>
+  <si>
+    <t>Flowserve</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Acessos</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Cteep</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>observacao</t>
   </si>
 </sst>
 </file>
@@ -105,13 +126,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,40 +433,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -460,107 +470,72 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2">
+        <v>321</v>
+      </c>
+      <c r="F2">
+        <v>123234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Alteração no CSS para melhor enquadramento de div
</commit_message>
<xml_diff>
--- a/monitorias.xlsx
+++ b/monitorias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-04-24</t>
+          <t>2024-04-28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -497,19 +497,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="D2" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="E2" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="F2" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="G2" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -517,59 +517,1733 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="J2" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-04-24</t>
+          <t>2024-04-28</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>234</v>
+      </c>
+      <c r="D3" t="n">
+        <v>234</v>
+      </c>
+      <c r="E3" t="n">
+        <v>234</v>
+      </c>
+      <c r="F3" t="n">
+        <v>234</v>
+      </c>
+      <c r="G3" t="n">
+        <v>234</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>234</v>
+      </c>
+      <c r="J3" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>345</v>
+      </c>
+      <c r="D4" t="n">
+        <v>345</v>
+      </c>
+      <c r="E4" t="n">
+        <v>345</v>
+      </c>
+      <c r="F4" t="n">
+        <v>345</v>
+      </c>
+      <c r="G4" t="n">
+        <v>345</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>345</v>
+      </c>
+      <c r="J4" t="n">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>UUS</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Acessos</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>456</v>
+      </c>
+      <c r="D5" t="n">
+        <v>456</v>
+      </c>
+      <c r="E5" t="n">
+        <v>456</v>
+      </c>
+      <c r="F5" t="n">
+        <v>456</v>
+      </c>
+      <c r="G5" t="n">
+        <v>456</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Consulta</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>456</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>45</v>
+      </c>
+      <c r="D6" t="n">
+        <v>45</v>
+      </c>
+      <c r="E6" t="n">
+        <v>45</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45</v>
+      </c>
+      <c r="G6" t="n">
+        <v>45</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Software</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>45</v>
+      </c>
+      <c r="J6" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>UUS</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>456</v>
+      </c>
+      <c r="D7" t="n">
+        <v>456</v>
+      </c>
+      <c r="E7" t="n">
+        <v>456</v>
+      </c>
+      <c r="F7" t="n">
+        <v>456</v>
+      </c>
+      <c r="G7" t="n">
+        <v>456</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>456</v>
+      </c>
+      <c r="J7" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>456</v>
+      </c>
+      <c r="D8" t="n">
+        <v>45</v>
+      </c>
+      <c r="E8" t="n">
+        <v>456</v>
+      </c>
+      <c r="F8" t="n">
+        <v>456</v>
+      </c>
+      <c r="G8" t="n">
+        <v>456</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>456</v>
+      </c>
+      <c r="J8" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>456</v>
+      </c>
+      <c r="D9" t="n">
+        <v>45</v>
+      </c>
+      <c r="E9" t="n">
+        <v>456</v>
+      </c>
+      <c r="F9" t="n">
+        <v>456</v>
+      </c>
+      <c r="G9" t="n">
+        <v>456</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>456</v>
+      </c>
+      <c r="J9" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>456</v>
+      </c>
+      <c r="D10" t="n">
+        <v>45</v>
+      </c>
+      <c r="E10" t="n">
+        <v>456</v>
+      </c>
+      <c r="F10" t="n">
+        <v>456</v>
+      </c>
+      <c r="G10" t="n">
+        <v>456</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>456</v>
+      </c>
+      <c r="J10" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>456</v>
+      </c>
+      <c r="D11" t="n">
+        <v>45</v>
+      </c>
+      <c r="E11" t="n">
+        <v>456</v>
+      </c>
+      <c r="F11" t="n">
+        <v>456</v>
+      </c>
+      <c r="G11" t="n">
+        <v>456</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>456</v>
+      </c>
+      <c r="J11" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>456</v>
+      </c>
+      <c r="D12" t="n">
+        <v>45</v>
+      </c>
+      <c r="E12" t="n">
+        <v>456</v>
+      </c>
+      <c r="F12" t="n">
+        <v>456</v>
+      </c>
+      <c r="G12" t="n">
+        <v>456</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>456</v>
+      </c>
+      <c r="J12" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>456</v>
+      </c>
+      <c r="D13" t="n">
+        <v>45</v>
+      </c>
+      <c r="E13" t="n">
+        <v>456</v>
+      </c>
+      <c r="F13" t="n">
+        <v>456</v>
+      </c>
+      <c r="G13" t="n">
+        <v>456</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>456</v>
+      </c>
+      <c r="J13" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>456</v>
+      </c>
+      <c r="D14" t="n">
+        <v>45</v>
+      </c>
+      <c r="E14" t="n">
+        <v>456</v>
+      </c>
+      <c r="F14" t="n">
+        <v>456</v>
+      </c>
+      <c r="G14" t="n">
+        <v>456</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>456</v>
+      </c>
+      <c r="J14" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>456</v>
+      </c>
+      <c r="D15" t="n">
+        <v>45</v>
+      </c>
+      <c r="E15" t="n">
+        <v>456</v>
+      </c>
+      <c r="F15" t="n">
+        <v>456</v>
+      </c>
+      <c r="G15" t="n">
+        <v>456</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>456</v>
+      </c>
+      <c r="J15" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>456</v>
+      </c>
+      <c r="D16" t="n">
+        <v>45</v>
+      </c>
+      <c r="E16" t="n">
+        <v>456</v>
+      </c>
+      <c r="F16" t="n">
+        <v>456</v>
+      </c>
+      <c r="G16" t="n">
+        <v>456</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>456</v>
+      </c>
+      <c r="J16" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>456</v>
+      </c>
+      <c r="D17" t="n">
+        <v>45</v>
+      </c>
+      <c r="E17" t="n">
+        <v>456</v>
+      </c>
+      <c r="F17" t="n">
+        <v>456</v>
+      </c>
+      <c r="G17" t="n">
+        <v>456</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>456</v>
+      </c>
+      <c r="J17" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>456</v>
+      </c>
+      <c r="D18" t="n">
+        <v>45</v>
+      </c>
+      <c r="E18" t="n">
+        <v>456</v>
+      </c>
+      <c r="F18" t="n">
+        <v>456</v>
+      </c>
+      <c r="G18" t="n">
+        <v>456</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>456</v>
+      </c>
+      <c r="J18" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>456</v>
+      </c>
+      <c r="D19" t="n">
+        <v>45</v>
+      </c>
+      <c r="E19" t="n">
+        <v>456</v>
+      </c>
+      <c r="F19" t="n">
+        <v>456</v>
+      </c>
+      <c r="G19" t="n">
+        <v>456</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>456</v>
+      </c>
+      <c r="J19" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>456</v>
+      </c>
+      <c r="D20" t="n">
+        <v>45</v>
+      </c>
+      <c r="E20" t="n">
+        <v>456</v>
+      </c>
+      <c r="F20" t="n">
+        <v>456</v>
+      </c>
+      <c r="G20" t="n">
+        <v>456</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>456</v>
+      </c>
+      <c r="J20" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>456</v>
+      </c>
+      <c r="D21" t="n">
+        <v>45</v>
+      </c>
+      <c r="E21" t="n">
+        <v>456</v>
+      </c>
+      <c r="F21" t="n">
+        <v>456</v>
+      </c>
+      <c r="G21" t="n">
+        <v>456</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>456</v>
+      </c>
+      <c r="J21" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>456</v>
+      </c>
+      <c r="D22" t="n">
+        <v>45</v>
+      </c>
+      <c r="E22" t="n">
+        <v>456</v>
+      </c>
+      <c r="F22" t="n">
+        <v>456</v>
+      </c>
+      <c r="G22" t="n">
+        <v>456</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>456</v>
+      </c>
+      <c r="J22" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>456</v>
+      </c>
+      <c r="D23" t="n">
+        <v>45</v>
+      </c>
+      <c r="E23" t="n">
+        <v>456</v>
+      </c>
+      <c r="F23" t="n">
+        <v>456</v>
+      </c>
+      <c r="G23" t="n">
+        <v>456</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>456</v>
+      </c>
+      <c r="J23" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>456</v>
+      </c>
+      <c r="D24" t="n">
+        <v>45</v>
+      </c>
+      <c r="E24" t="n">
+        <v>456</v>
+      </c>
+      <c r="F24" t="n">
+        <v>456</v>
+      </c>
+      <c r="G24" t="n">
+        <v>456</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>456</v>
+      </c>
+      <c r="J24" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>456</v>
+      </c>
+      <c r="D25" t="n">
+        <v>45</v>
+      </c>
+      <c r="E25" t="n">
+        <v>456</v>
+      </c>
+      <c r="F25" t="n">
+        <v>456</v>
+      </c>
+      <c r="G25" t="n">
+        <v>456</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>456</v>
+      </c>
+      <c r="J25" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>456</v>
+      </c>
+      <c r="D26" t="n">
+        <v>45</v>
+      </c>
+      <c r="E26" t="n">
+        <v>456</v>
+      </c>
+      <c r="F26" t="n">
+        <v>456</v>
+      </c>
+      <c r="G26" t="n">
+        <v>456</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>456</v>
+      </c>
+      <c r="J26" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>456</v>
+      </c>
+      <c r="D27" t="n">
+        <v>45</v>
+      </c>
+      <c r="E27" t="n">
+        <v>456</v>
+      </c>
+      <c r="F27" t="n">
+        <v>456</v>
+      </c>
+      <c r="G27" t="n">
+        <v>456</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>456</v>
+      </c>
+      <c r="J27" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>456</v>
+      </c>
+      <c r="D28" t="n">
+        <v>45</v>
+      </c>
+      <c r="E28" t="n">
+        <v>456</v>
+      </c>
+      <c r="F28" t="n">
+        <v>456</v>
+      </c>
+      <c r="G28" t="n">
+        <v>456</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>456</v>
+      </c>
+      <c r="J28" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>456</v>
+      </c>
+      <c r="D29" t="n">
+        <v>45</v>
+      </c>
+      <c r="E29" t="n">
+        <v>456</v>
+      </c>
+      <c r="F29" t="n">
+        <v>456</v>
+      </c>
+      <c r="G29" t="n">
+        <v>456</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>456</v>
+      </c>
+      <c r="J29" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>456</v>
+      </c>
+      <c r="D30" t="n">
+        <v>45</v>
+      </c>
+      <c r="E30" t="n">
+        <v>456</v>
+      </c>
+      <c r="F30" t="n">
+        <v>456</v>
+      </c>
+      <c r="G30" t="n">
+        <v>456</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>456</v>
+      </c>
+      <c r="J30" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>456</v>
+      </c>
+      <c r="D31" t="n">
+        <v>45</v>
+      </c>
+      <c r="E31" t="n">
+        <v>456</v>
+      </c>
+      <c r="F31" t="n">
+        <v>456</v>
+      </c>
+      <c r="G31" t="n">
+        <v>456</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>456</v>
+      </c>
+      <c r="J31" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>456</v>
+      </c>
+      <c r="D32" t="n">
+        <v>45</v>
+      </c>
+      <c r="E32" t="n">
+        <v>456</v>
+      </c>
+      <c r="F32" t="n">
+        <v>456</v>
+      </c>
+      <c r="G32" t="n">
+        <v>456</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>456</v>
+      </c>
+      <c r="J32" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>456</v>
+      </c>
+      <c r="D33" t="n">
+        <v>45</v>
+      </c>
+      <c r="E33" t="n">
+        <v>456</v>
+      </c>
+      <c r="F33" t="n">
+        <v>456</v>
+      </c>
+      <c r="G33" t="n">
+        <v>456</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>456</v>
+      </c>
+      <c r="J33" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>456</v>
+      </c>
+      <c r="D34" t="n">
+        <v>45</v>
+      </c>
+      <c r="E34" t="n">
+        <v>456</v>
+      </c>
+      <c r="F34" t="n">
+        <v>456</v>
+      </c>
+      <c r="G34" t="n">
+        <v>456</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>456</v>
+      </c>
+      <c r="J34" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>456</v>
+      </c>
+      <c r="D35" t="n">
+        <v>45</v>
+      </c>
+      <c r="E35" t="n">
+        <v>456</v>
+      </c>
+      <c r="F35" t="n">
+        <v>456</v>
+      </c>
+      <c r="G35" t="n">
+        <v>456</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>456</v>
+      </c>
+      <c r="J35" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>456</v>
+      </c>
+      <c r="D36" t="n">
+        <v>45</v>
+      </c>
+      <c r="E36" t="n">
+        <v>456</v>
+      </c>
+      <c r="F36" t="n">
+        <v>456</v>
+      </c>
+      <c r="G36" t="n">
+        <v>456</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>456</v>
+      </c>
+      <c r="J36" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>456</v>
+      </c>
+      <c r="D37" t="n">
+        <v>45</v>
+      </c>
+      <c r="E37" t="n">
+        <v>456</v>
+      </c>
+      <c r="F37" t="n">
+        <v>456</v>
+      </c>
+      <c r="G37" t="n">
+        <v>456</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>456</v>
+      </c>
+      <c r="J37" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>456</v>
+      </c>
+      <c r="D38" t="n">
+        <v>45</v>
+      </c>
+      <c r="E38" t="n">
+        <v>456</v>
+      </c>
+      <c r="F38" t="n">
+        <v>456</v>
+      </c>
+      <c r="G38" t="n">
+        <v>456</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>456</v>
+      </c>
+      <c r="J38" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>456</v>
+      </c>
+      <c r="D39" t="n">
+        <v>45</v>
+      </c>
+      <c r="E39" t="n">
+        <v>456</v>
+      </c>
+      <c r="F39" t="n">
+        <v>456</v>
+      </c>
+      <c r="G39" t="n">
+        <v>456</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>456</v>
+      </c>
+      <c r="J39" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>456</v>
+      </c>
+      <c r="D40" t="n">
+        <v>45</v>
+      </c>
+      <c r="E40" t="n">
+        <v>456</v>
+      </c>
+      <c r="F40" t="n">
+        <v>456</v>
+      </c>
+      <c r="G40" t="n">
+        <v>456</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>456</v>
+      </c>
+      <c r="J40" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>456</v>
+      </c>
+      <c r="D41" t="n">
+        <v>45</v>
+      </c>
+      <c r="E41" t="n">
+        <v>456</v>
+      </c>
+      <c r="F41" t="n">
+        <v>456</v>
+      </c>
+      <c r="G41" t="n">
+        <v>456</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>456</v>
+      </c>
+      <c r="J41" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>456</v>
+      </c>
+      <c r="D42" t="n">
+        <v>45</v>
+      </c>
+      <c r="E42" t="n">
+        <v>456</v>
+      </c>
+      <c r="F42" t="n">
+        <v>456</v>
+      </c>
+      <c r="G42" t="n">
+        <v>456</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>456</v>
+      </c>
+      <c r="J42" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>456</v>
+      </c>
+      <c r="D43" t="n">
+        <v>45</v>
+      </c>
+      <c r="E43" t="n">
+        <v>456</v>
+      </c>
+      <c r="F43" t="n">
+        <v>456</v>
+      </c>
+      <c r="G43" t="n">
+        <v>456</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>456</v>
+      </c>
+      <c r="J43" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>456</v>
+      </c>
+      <c r="D44" t="n">
+        <v>45</v>
+      </c>
+      <c r="E44" t="n">
+        <v>456</v>
+      </c>
+      <c r="F44" t="n">
+        <v>456</v>
+      </c>
+      <c r="G44" t="n">
+        <v>456</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>456</v>
+      </c>
+      <c r="J44" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>456</v>
+      </c>
+      <c r="D45" t="n">
+        <v>45</v>
+      </c>
+      <c r="E45" t="n">
+        <v>456</v>
+      </c>
+      <c r="F45" t="n">
+        <v>456</v>
+      </c>
+      <c r="G45" t="n">
+        <v>456</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>456</v>
+      </c>
+      <c r="J45" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>456</v>
+      </c>
+      <c r="D46" t="n">
+        <v>45</v>
+      </c>
+      <c r="E46" t="n">
+        <v>456</v>
+      </c>
+      <c r="F46" t="n">
+        <v>456</v>
+      </c>
+      <c r="G46" t="n">
+        <v>456</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>456</v>
+      </c>
+      <c r="J46" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>34345</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>3453</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Software</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>34535</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
melhorias na tabela e estilo do form
</commit_message>
<xml_diff>
--- a/monitorias.xlsx
+++ b/monitorias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2204,44 +2204,303 @@
           <t>Cteep</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>34345</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>3453</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>345</t>
-        </is>
+      <c r="C47" t="n">
+        <v>34345</v>
+      </c>
+      <c r="D47" t="n">
+        <v>3453</v>
+      </c>
+      <c r="E47" t="n">
+        <v>34</v>
+      </c>
+      <c r="F47" t="n">
+        <v>34</v>
+      </c>
+      <c r="G47" t="n">
+        <v>345</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
           <t>Software</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>345</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>34535</t>
+      <c r="I47" t="n">
+        <v>345</v>
+      </c>
+      <c r="J47" t="n">
+        <v>34535</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>UUS</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>111</v>
+      </c>
+      <c r="D49" t="n">
+        <v>111</v>
+      </c>
+      <c r="E49" t="n">
+        <v>111</v>
+      </c>
+      <c r="F49" t="n">
+        <v>111</v>
+      </c>
+      <c r="G49" t="n">
+        <v>111</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>123</v>
+      </c>
+      <c r="J49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Guilherme Ribas</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>12312312312</v>
+      </c>
+      <c r="E50" t="n">
+        <v>123</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1231312312</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>JOSE BENETIDO DOS SANTOS PINHEIRO DA SILVA JUNIOR</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Hardware</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>100</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>123</v>
+      </c>
+      <c r="E51" t="n">
+        <v>123</v>
+      </c>
+      <c r="F51" t="n">
+        <v>123</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>123</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa
+aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa
+aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa
+aaaaaaaaaaaa
+a
+a
+a
+a
+aa
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a
+a</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
alteração na mensagem de confirmação
</commit_message>
<xml_diff>
--- a/monitorias.xlsx
+++ b/monitorias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2426,35 +2426,27 @@
           <t>a</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H52" t="inlineStr">
         <is>
           <t>Acessos</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="I52" t="n">
+        <v>1</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -2501,6 +2493,749 @@
 a
 a
 a</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-04-28</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>123</v>
+      </c>
+      <c r="F53" t="n">
+        <v>123</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>123</v>
+      </c>
+      <c r="J53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-04-22</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>333</v>
+      </c>
+      <c r="F54" t="n">
+        <v>333</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>333</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>123</v>
+      </c>
+      <c r="F55" t="n">
+        <v>123</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>123</v>
+      </c>
+      <c r="J55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>123</v>
+      </c>
+      <c r="F56" t="n">
+        <v>123</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>123</v>
+      </c>
+      <c r="J56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>123</v>
+      </c>
+      <c r="F57" t="n">
+        <v>123</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>123</v>
+      </c>
+      <c r="J57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>123</v>
+      </c>
+      <c r="F58" t="n">
+        <v>123</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>123</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>123</v>
+      </c>
+      <c r="F59" t="n">
+        <v>123</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>123</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>123</v>
+      </c>
+      <c r="F60" t="n">
+        <v>123</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>12</v>
+      </c>
+      <c r="J60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>234</v>
+      </c>
+      <c r="F61" t="n">
+        <v>234</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>23</v>
+      </c>
+      <c r="J61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>123</v>
+      </c>
+      <c r="F62" t="n">
+        <v>123</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>123</v>
+      </c>
+      <c r="J62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>123</v>
+      </c>
+      <c r="F63" t="n">
+        <v>132</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>123</v>
+      </c>
+      <c r="J63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>123</v>
+      </c>
+      <c r="F64" t="n">
+        <v>123</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>123</v>
+      </c>
+      <c r="J64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Henkel</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>123</v>
+      </c>
+      <c r="F65" t="n">
+        <v>13</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>13</v>
+      </c>
+      <c r="J65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>123</v>
+      </c>
+      <c r="F66" t="n">
+        <v>123</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>123</v>
+      </c>
+      <c r="J66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>wer</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>234</v>
+      </c>
+      <c r="F67" t="n">
+        <v>234</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>234</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">234
+234
+234
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>123</v>
+      </c>
+      <c r="F68" t="n">
+        <v>123</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>123</v>
+      </c>
+      <c r="J68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Cteep</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>123</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
estrutura da pasta static
</commit_message>
<xml_diff>
--- a/monitorias.xlsx
+++ b/monitorias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3300,15 +3300,11 @@
           <t>f</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>213</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
+      <c r="E71" t="n">
+        <v>213</v>
+      </c>
+      <c r="F71" t="n">
+        <v>123</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -3320,16 +3316,62 @@
           <t>Acessos</t>
         </is>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>345</t>
-        </is>
+      <c r="I71" t="n">
+        <v>345</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
           <t>dszfs</t>
         </is>
       </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-04-30</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Flowserve</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Acessos</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>